<commit_message>
modified fpc name | with push.sh V1.3
</commit_message>
<xml_diff>
--- a/BOM V1.xlsx
+++ b/BOM V1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView/>
+    <workbookView windowWidth="14688" windowHeight="13535"/>
   </bookViews>
   <sheets>
     <sheet name="BOM V1" sheetId="1" r:id="rId1"/>
@@ -461,10 +461,17 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -614,7 +621,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -624,6 +631,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD3D3D3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1108,10 +1121,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1120,36 +1133,33 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1159,98 +1169,101 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1282,12 +1295,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
@@ -1306,12 +1325,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" quotePrefix="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" quotePrefix="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" quotePrefix="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" quotePrefix="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" quotePrefix="1">
@@ -1638,13 +1663,15 @@
   <sheetPr/>
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="6" width="19.0277777777778" customWidth="1"/>
+    <col min="1" max="2" width="19.0277777777778" customWidth="1"/>
+    <col min="3" max="3" width="35.6296296296296" customWidth="1"/>
+    <col min="4" max="6" width="19.0277777777778" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" spans="1:6">
@@ -1668,19 +1695,19 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="18" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="7">
@@ -1688,19 +1715,19 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="20" t="s">
         <v>15</v>
       </c>
       <c r="F3" s="10">
@@ -1708,19 +1735,19 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="20" t="s">
         <v>15</v>
       </c>
       <c r="F4" s="10">
@@ -1728,19 +1755,19 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="20" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="10">
@@ -1748,19 +1775,19 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="20" t="s">
         <v>15</v>
       </c>
       <c r="F6" s="10">
@@ -1768,19 +1795,19 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="20" t="s">
         <v>15</v>
       </c>
       <c r="F7" s="10">
@@ -1788,19 +1815,19 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="20" t="s">
         <v>15</v>
       </c>
       <c r="F8" s="10">
@@ -1808,19 +1835,19 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="20" t="s">
         <v>15</v>
       </c>
       <c r="F9" s="10">
@@ -1828,19 +1855,19 @@
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="20" t="s">
         <v>32</v>
       </c>
       <c r="F10" s="10">
@@ -1848,19 +1875,19 @@
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="D11" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="20" t="s">
         <v>32</v>
       </c>
       <c r="F11" s="10">
@@ -1868,19 +1895,19 @@
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="20" t="s">
         <v>36</v>
       </c>
       <c r="F12" s="10">
@@ -1888,19 +1915,19 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="18" t="s">
+      <c r="E13" s="20" t="s">
         <v>44</v>
       </c>
       <c r="F13" s="10">
@@ -1908,19 +1935,19 @@
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="20" t="s">
         <v>44</v>
       </c>
       <c r="F14" s="10">
@@ -1928,19 +1955,19 @@
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="18" t="s">
+      <c r="E15" s="20" t="s">
         <v>44</v>
       </c>
       <c r="F15" s="10">
@@ -1948,19 +1975,19 @@
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="E16" s="20" t="s">
         <v>44</v>
       </c>
       <c r="F16" s="10">
@@ -1968,19 +1995,19 @@
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="20" t="s">
         <v>44</v>
       </c>
       <c r="F17" s="10">
@@ -1988,19 +2015,19 @@
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="18" t="s">
+      <c r="D18" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="E18" s="18" t="s">
+      <c r="E18" s="20" t="s">
         <v>44</v>
       </c>
       <c r="F18" s="10">
@@ -2008,19 +2035,19 @@
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="18" t="s">
+      <c r="C19" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="20" t="s">
         <v>44</v>
       </c>
       <c r="F19" s="10">
@@ -2028,19 +2055,19 @@
       </c>
     </row>
     <row r="20" ht="158.4" spans="1:6">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="D20" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="E20" s="18" t="s">
+      <c r="E20" s="20" t="s">
         <v>57</v>
       </c>
       <c r="F20" s="10">
@@ -2048,19 +2075,19 @@
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="D21" s="18" t="s">
+      <c r="D21" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="18" t="s">
+      <c r="E21" s="20" t="s">
         <v>65</v>
       </c>
       <c r="F21" s="10">
@@ -2068,19 +2095,19 @@
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D22" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E22" s="18" t="s">
+      <c r="E22" s="20" t="s">
         <v>66</v>
       </c>
       <c r="F22" s="10">
@@ -2088,19 +2115,19 @@
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="B23" s="18" t="s">
+      <c r="B23" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="E23" s="18" t="s">
+      <c r="E23" s="20" t="s">
         <v>70</v>
       </c>
       <c r="F23" s="10">
@@ -2108,19 +2135,19 @@
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D24" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="E24" s="18" t="s">
+      <c r="E24" s="20" t="s">
         <v>77</v>
       </c>
       <c r="F24" s="10">
@@ -2128,19 +2155,19 @@
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="D25" s="18" t="s">
+      <c r="D25" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="E25" s="18" t="s">
+      <c r="E25" s="20" t="s">
         <v>78</v>
       </c>
       <c r="F25" s="10">
@@ -2148,19 +2175,19 @@
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="D26" s="18" t="s">
+      <c r="D26" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="E26" s="18" t="s">
+      <c r="E26" s="20" t="s">
         <v>86</v>
       </c>
       <c r="F26" s="10">
@@ -2168,19 +2195,19 @@
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="C27" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="E27" s="18" t="s">
+      <c r="E27" s="20" t="s">
         <v>91</v>
       </c>
       <c r="F27" s="10">
@@ -2188,19 +2215,19 @@
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="C28" s="18" t="s">
+      <c r="C28" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="D28" s="18" t="s">
+      <c r="D28" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="E28" s="18" t="s">
+      <c r="E28" s="20" t="s">
         <v>91</v>
       </c>
       <c r="F28" s="10">
@@ -2208,19 +2235,19 @@
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="17" t="s">
+      <c r="A29" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="C29" s="18" t="s">
+      <c r="C29" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="D29" s="18" t="s">
+      <c r="D29" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="E29" s="18" t="s">
+      <c r="E29" s="20" t="s">
         <v>94</v>
       </c>
       <c r="F29" s="10">
@@ -2228,19 +2255,19 @@
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="17" t="s">
+      <c r="A30" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="C30" s="18" t="s">
+      <c r="C30" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="D30" s="18" t="s">
+      <c r="D30" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="E30" s="18" t="s">
+      <c r="E30" s="20" t="s">
         <v>98</v>
       </c>
       <c r="F30" s="10">
@@ -2248,19 +2275,19 @@
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="17" t="s">
+      <c r="A31" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="C31" s="18" t="s">
+      <c r="C31" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="D31" s="18" t="s">
+      <c r="D31" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="E31" s="18" t="s">
+      <c r="E31" s="20" t="s">
         <v>106</v>
       </c>
       <c r="F31" s="10">
@@ -2268,19 +2295,19 @@
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="D32" s="18" t="s">
+      <c r="D32" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="E32" s="18" t="s">
+      <c r="E32" s="20" t="s">
         <v>15</v>
       </c>
       <c r="F32" s="10">
@@ -2288,19 +2315,19 @@
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="17" t="s">
+      <c r="A33" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="B33" s="18" t="s">
+      <c r="B33" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="C33" s="18" t="s">
+      <c r="C33" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="D33" s="18" t="s">
+      <c r="D33" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="E33" s="18" t="s">
+      <c r="E33" s="20" t="s">
         <v>111</v>
       </c>
       <c r="F33" s="10">
@@ -2308,19 +2335,19 @@
       </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="17" t="s">
+      <c r="A34" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="C34" s="18" t="s">
+      <c r="C34" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="D34" s="18" t="s">
+      <c r="D34" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="E34" s="18" t="s">
+      <c r="E34" s="20" t="s">
         <v>119</v>
       </c>
       <c r="F34" s="10">
@@ -2328,19 +2355,19 @@
       </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="17" t="s">
+      <c r="A35" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="C35" s="18" t="s">
+      <c r="C35" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="D35" s="18" t="s">
+      <c r="D35" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="E35" s="18" t="s">
+      <c r="E35" s="20" t="s">
         <v>124</v>
       </c>
       <c r="F35" s="10">
@@ -2348,19 +2375,19 @@
       </c>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="17" t="s">
+      <c r="A36" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="C36" s="18" t="s">
+      <c r="C36" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="D36" s="18" t="s">
+      <c r="D36" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="E36" s="18" t="s">
+      <c r="E36" s="20" t="s">
         <v>129</v>
       </c>
       <c r="F36" s="10">
@@ -2368,19 +2395,19 @@
       </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="17" t="s">
+      <c r="A37" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="B37" s="18" t="s">
+      <c r="B37" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="C37" s="18" t="s">
+      <c r="C37" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="D37" s="18" t="s">
+      <c r="D37" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="E37" s="18" t="s">
+      <c r="E37" s="20" t="s">
         <v>129</v>
       </c>
       <c r="F37" s="10">
@@ -2388,19 +2415,19 @@
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="17" t="s">
+      <c r="A38" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="B38" s="18" t="s">
+      <c r="B38" s="20" t="s">
         <v>132</v>
       </c>
-      <c r="C38" s="18" t="s">
+      <c r="C38" s="20" t="s">
         <v>133</v>
       </c>
-      <c r="D38" s="18" t="s">
+      <c r="D38" s="20" t="s">
         <v>134</v>
       </c>
-      <c r="E38" s="18" t="s">
+      <c r="E38" s="20" t="s">
         <v>135</v>
       </c>
       <c r="F38" s="10">
@@ -2408,19 +2435,19 @@
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="17" t="s">
+      <c r="A39" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="B39" s="18" t="s">
+      <c r="B39" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="C39" s="18" t="s">
+      <c r="C39" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="D39" s="18" t="s">
+      <c r="D39" s="20" t="s">
         <v>139</v>
       </c>
-      <c r="E39" s="18" t="s">
+      <c r="E39" s="20" t="s">
         <v>140</v>
       </c>
       <c r="F39" s="10">
@@ -2428,22 +2455,22 @@
       </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="20" t="s">
+      <c r="A40" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="B40" s="21" t="s">
+      <c r="B40" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="C40" s="21" t="s">
+      <c r="C40" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="D40" s="21" t="s">
+      <c r="D40" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="E40" s="21" t="s">
+      <c r="E40" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="F40" s="14">
+      <c r="F40" s="16">
         <v>1</v>
       </c>
     </row>

</xml_diff>